<commit_message>
Updated ReadMe.xlsx to get idea about framework layers.
</commit_message>
<xml_diff>
--- a/ReadMe.xlsx
+++ b/ReadMe.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DEAF2A-4EFD-4715-8F4E-44A33417016B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>StandardUtilities</t>
   </si>
@@ -55,9 +56,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Coded UI Support</t>
-  </si>
-  <si>
     <t>Debasish Pradhan</t>
   </si>
   <si>
@@ -68,30 +66,6 @@
   </si>
   <si>
     <t>Excel Data Reading</t>
-  </si>
-  <si>
-    <t>Database Reading</t>
-  </si>
-  <si>
-    <t>Parallel Execution</t>
-  </si>
-  <si>
-    <t>Cloud Support</t>
-  </si>
-  <si>
-    <t>Sushmitha</t>
-  </si>
-  <si>
-    <t>Ashish</t>
-  </si>
-  <si>
-    <t>Swarup</t>
-  </si>
-  <si>
-    <t>Sriram</t>
-  </si>
-  <si>
-    <t>Panigrahi</t>
   </si>
   <si>
     <t>Framework Layers</t>
@@ -125,11 +99,32 @@
   <si>
     <t>This is the loosely coupled test layer which does actual testing. It uses the services of other layers -TestReporter/AUT/Engine/StandardUtilities.</t>
   </si>
+  <si>
+    <t>Test Rail Support</t>
+  </si>
+  <si>
+    <t>Mail Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug and Play Third Party Test Execution Report </t>
+  </si>
+  <si>
+    <t>Log4Net</t>
+  </si>
+  <si>
+    <t>Jenkins Support</t>
+  </si>
+  <si>
+    <t>TestRail</t>
+  </si>
+  <si>
+    <t>This rail use gurock test rail APIs to communicate with TestRail to update test case status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -333,19 +328,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -369,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,6 +362,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -389,92 +449,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,22 +477,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>333376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2562225</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>742949</xdr:rowOff>
+      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D1BA75E-3DEC-4521-8F41-ED0CE1EF428A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30814BF5-F097-4B9D-B114-AFBD8FFDFE4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -529,8 +508,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7934325" y="1343024"/>
-          <a:ext cx="2085975" cy="2733675"/>
+          <a:off x="7705725" y="1190626"/>
+          <a:ext cx="2419350" cy="3228974"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -838,211 +817,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="25">
-        <v>42276</v>
+      <c r="D3" s="19">
+        <v>43385</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="17">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="28">
-        <v>42289</v>
+      <c r="C4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="19">
+        <v>43416</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="17">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="28">
-        <v>42320</v>
+      <c r="C5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="19">
+        <v>43419</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="17">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="28">
-        <v>42323</v>
+      <c r="B6" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="19">
+        <v>43452</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="A7" s="17">
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="28">
-        <v>42401</v>
+      <c r="B7" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="34">
+        <v>43525</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="17">
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="28">
-        <v>42412</v>
+      <c r="B8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="34">
+        <v>43575</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+      <c r="A9" s="17">
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="28">
-        <v>42510</v>
+      <c r="B9" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="19">
+        <v>43804</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="29"/>
+      <c r="A10" s="17">
+        <v>8</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="19">
+        <v>43814</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="29"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="29"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="29"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="29"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="29"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="29"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="29"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1054,11 +1023,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,114 +1040,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>26</v>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="29"/>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="29"/>
+    </row>
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="34"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="34"/>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="34"/>
-    </row>
-    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="34"/>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="34"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="34"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="33"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="33"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="35"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
All Test Case Running In Single Thread And EMAIL Configured With GMAIL SMTP With debasish.gallop id.
</commit_message>
<xml_diff>
--- a/ReadMe.xlsx
+++ b/ReadMe.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DEAF2A-4EFD-4715-8F4E-44A33417016B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF40169-3C69-4068-92D2-04F0D0FDA9E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,14 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>StandardUtilities</t>
   </si>
   <si>
-    <t>GallopReporter</t>
-  </si>
-  <si>
     <t>TestReporter</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>Responsibilities</t>
-  </si>
-  <si>
-    <t>Gallop Specific Html Report. Gallop Reporter is intellectual property of Gallop.</t>
   </si>
   <si>
     <t>The layer provides interfaces which can be seamlessly used to integrate any third party reporting framework. Currently, this layer integrates GallopReporter (Gallop IP reporting framework)/ExtentReport (third party reporting framework)</t>
@@ -115,10 +109,22 @@
     <t>Jenkins Support</t>
   </si>
   <si>
-    <t>TestRail</t>
-  </si>
-  <si>
-    <t>This rail use gurock test rail APIs to communicate with TestRail to update test case status</t>
+    <t>CignitiReporter</t>
+  </si>
+  <si>
+    <t>Cigniti Specific Html Report. Cigniti Reporter is intellectual property of Cigniti.</t>
+  </si>
+  <si>
+    <t>TMTFactory</t>
+  </si>
+  <si>
+    <t>Implementation Of Test Rail API's to operate on Test Rail Objects such as Test Case Status Update, Reading Project/Suite/Run information.</t>
+  </si>
+  <si>
+    <t>TCM Factory</t>
+  </si>
+  <si>
+    <t>Designing data structure for Test Cases to store test case related information and operate test case data for reporting purpose.</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -342,6 +348,75 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -359,74 +434,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -440,20 +494,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,22 +552,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>333376</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:colOff>2695575</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:rowOff>911392</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30814BF5-F097-4B9D-B114-AFBD8FFDFE4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A06C603-F89B-4F2F-9AEF-EEBD17A21BDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -508,8 +583,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7705725" y="1190626"/>
-          <a:ext cx="2419350" cy="3228974"/>
+          <a:off x="7696200" y="914400"/>
+          <a:ext cx="2457450" cy="2759242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -832,168 +907,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="33" t="s">
+      <c r="D3" s="12">
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="19">
-        <v>43385</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>2</v>
-      </c>
-      <c r="B4" s="33" t="s">
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="12">
+        <v>43416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="19">
-        <v>43416</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>3</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="19">
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12">
         <v>43419</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="12">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="18">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="18">
+        <v>43575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="12">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19">
-        <v>43452</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>5</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="34">
-        <v>43525</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>6</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="34">
-        <v>43575</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>7</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="19">
-        <v>43804</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>8</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="19">
+      <c r="C10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12">
         <v>43814</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="20"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="20"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="20"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1024,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,125 +1114,125 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="31"/>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="29"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="29"/>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="C10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="29"/>
-    </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="29"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="24"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="25"/>
+      <c r="D10" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="D3:D10"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>